<commit_message>
checking pool for nohome - , address for noaddress
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -218,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -249,12 +249,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -311,7 +305,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -335,14 +329,14 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.19"/>
   </cols>
@@ -778,6 +772,9 @@
       </c>
       <c r="G20" s="0" t="s">
         <v>59</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>